<commit_message>
Fixed softlock if the HQ was in a bad square
</commit_message>
<xml_diff>
--- a/MessagesIndex.xlsx
+++ b/MessagesIndex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\Documents\GitHub\Battlecode2023nullptr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACEEEE6-D5FE-4AAA-AC04-5D01FB657847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDAD5BF-3011-4134-924B-0B788877B6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t>Message ID</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Y-Coordinate</t>
   </si>
   <si>
-    <t>LOI ID</t>
-  </si>
-  <si>
     <t>Plot Origin</t>
   </si>
   <si>
@@ -60,18 +57,9 @@
     <t>Plot Block is always below the "Plot Origin" message.</t>
   </si>
   <si>
-    <t>Plot ID</t>
-  </si>
-  <si>
     <t>LRUD</t>
   </si>
   <si>
-    <t>Done?</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
     <t>Fourth</t>
   </si>
   <si>
@@ -94,13 +82,28 @@
   </si>
   <si>
     <t>Carrier?</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>Launch?</t>
+  </si>
+  <si>
+    <t>L/Dest?</t>
+  </si>
+  <si>
+    <t>Amp?</t>
+  </si>
+  <si>
+    <t>Cloud ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,19 +111,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -149,36 +139,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -204,6 +170,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -220,43 +210,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -266,6 +251,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF66FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -540,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,241 +603,275 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="2" t="s">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>101</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="8" t="s">
-        <v>13</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>100</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>101</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>110</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="9" t="s">
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="9"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>111</v>
+      </c>
+      <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>111</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>10</v>
+      <c r="C16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="C2:E9"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="K3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="K5:O5"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="K4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="P7:Q7"/>
+  <mergeCells count="26">
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="L6:Q6"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="L4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="F10:K10"/>
+    <mergeCell ref="L10:Q10"/>
+    <mergeCell ref="F8:K8"/>
+    <mergeCell ref="L8:Q8"/>
+    <mergeCell ref="J11:N11"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="P16:R16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>